<commit_message>
Fix text formatting of charts.
</commit_message>
<xml_diff>
--- a/PerformanceTestsResults.xls.xlsx
+++ b/PerformanceTestsResults.xls.xlsx
@@ -1171,7 +1171,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1179,7 +1179,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Cartesian Product</a:t>
             </a:r>
           </a:p>
@@ -1200,7 +1204,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1282,7 +1286,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1412,7 +1416,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1542,7 +1546,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1675,7 +1679,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1808,7 +1812,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1899,10 +1903,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1918,7 +1919,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1926,7 +1927,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Framework</a:t>
                 </a:r>
               </a:p>
@@ -1947,7 +1952,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1966,10 +1971,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2015,7 +2017,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2023,7 +2025,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Score ops/s</a:t>
                 </a:r>
               </a:p>
@@ -2044,7 +2050,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2073,7 +2079,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2112,7 +2118,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2183,7 +2189,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2212,7 +2218,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2286,15 +2292,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2416,15 +2420,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2546,15 +2548,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2679,15 +2679,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2812,15 +2810,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2911,10 +2907,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2930,7 +2923,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2959,7 +2952,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2975,13 +2968,12 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2994,7 +2986,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3027,7 +3019,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3056,7 +3048,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3085,7 +3077,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3124,7 +3116,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3159,7 +3151,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3195,7 +3191,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3203,7 +3199,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>countsBySuit</a:t>
             </a:r>
           </a:p>
@@ -3224,7 +3224,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3306,7 +3306,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3436,7 +3436,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3566,7 +3566,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3699,7 +3699,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3832,7 +3832,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3923,10 +3923,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3942,7 +3939,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3950,7 +3947,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Framework</a:t>
                 </a:r>
               </a:p>
@@ -3971,7 +3972,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3990,10 +3991,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4039,7 +4037,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4047,14 +4045,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Score</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t> ops/s</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4073,7 +4083,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -4102,7 +4112,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4141,7 +4151,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -4212,7 +4222,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4241,7 +4251,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -4315,15 +4325,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4445,15 +4453,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4575,15 +4581,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4708,15 +4712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4841,15 +4843,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4940,10 +4940,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4959,7 +4956,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4988,7 +4985,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -5007,10 +5004,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -5023,7 +5017,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -5056,7 +5050,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5085,7 +5079,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -5114,7 +5108,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -5153,7 +5147,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -5188,7 +5182,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -5224,7 +5222,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -5253,7 +5251,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -5327,15 +5325,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5457,15 +5453,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5587,15 +5581,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5720,15 +5712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5853,15 +5843,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -5952,10 +5940,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5971,7 +5956,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6000,7 +5985,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -6019,10 +6004,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -6035,7 +6017,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6068,7 +6050,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6097,7 +6079,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -6126,7 +6108,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6165,7 +6147,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -6200,7 +6182,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6236,7 +6222,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6265,7 +6251,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -6339,15 +6325,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6469,15 +6453,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6599,15 +6581,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6732,15 +6712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6865,15 +6843,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -6964,10 +6940,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6983,7 +6956,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7012,7 +6985,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -7031,10 +7004,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -7047,7 +7017,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -7080,7 +7050,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7109,7 +7079,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -7138,7 +7108,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -7177,7 +7147,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -7212,7 +7182,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -7248,7 +7222,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -7257,13 +7231,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Filter</a:t>
+              <a:t>Filter - List</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - List</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7282,7 +7251,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -7356,15 +7325,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7486,15 +7453,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7616,15 +7581,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7749,15 +7712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -7882,15 +7843,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8015,15 +7974,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8114,10 +8071,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -8133,7 +8087,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8162,7 +8116,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -8181,10 +8135,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -8197,7 +8148,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -8230,7 +8181,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8239,13 +8190,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Score</a:t>
+                  <a:t>Score ops/s</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> ops/s</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -8264,7 +8210,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -8293,7 +8239,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -8332,7 +8278,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -8367,7 +8313,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -8403,7 +8353,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -8432,7 +8382,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -8506,15 +8456,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8636,15 +8584,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8766,15 +8712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8899,15 +8843,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9032,15 +8974,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9165,15 +9105,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9264,10 +9202,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9283,7 +9218,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9312,7 +9247,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -9331,10 +9266,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -9347,7 +9279,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -9380,7 +9312,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9389,13 +9321,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Score</a:t>
+                  <a:t>Score ops/s</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> ops/s</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -9414,7 +9341,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -9443,7 +9370,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -9482,7 +9409,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -9517,7 +9444,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -9553,7 +9484,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -9582,7 +9513,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -9656,15 +9587,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9783,15 +9712,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -9913,15 +9840,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10046,15 +9971,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10179,15 +10102,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10312,15 +10233,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10411,10 +10330,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -10430,7 +10346,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10459,7 +10375,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -10475,13 +10391,12 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -10494,7 +10409,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -10527,7 +10442,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10536,13 +10451,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Score</a:t>
+                  <a:t>Score ops/s</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> ops/s</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -10561,7 +10471,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -10590,7 +10500,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -10629,7 +10539,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -10664,7 +10574,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -10700,7 +10614,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -10729,7 +10643,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -10803,15 +10717,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10933,15 +10845,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11063,15 +10973,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11196,15 +11104,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11329,15 +11235,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11462,15 +11366,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11561,10 +11463,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -11580,7 +11479,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11609,7 +11508,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -11628,10 +11527,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -11644,7 +11540,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -11677,7 +11573,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11706,7 +11602,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -11735,7 +11631,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -11774,7 +11670,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -11809,7 +11705,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -13056,7 +12956,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -13085,7 +12985,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -13159,15 +13059,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13289,15 +13187,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13419,15 +13315,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13552,15 +13446,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13685,15 +13577,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13818,15 +13708,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13917,10 +13805,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -13936,7 +13821,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13965,7 +13850,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -13984,10 +13869,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -14000,7 +13882,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -14033,7 +13915,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14062,7 +13944,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -14091,7 +13973,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -14130,7 +14012,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -14165,7 +14047,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -14201,7 +14087,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -14230,7 +14116,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -14304,15 +14190,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14431,15 +14315,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14561,15 +14443,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14694,15 +14574,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14827,15 +14705,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -14960,15 +14836,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -15059,10 +14933,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -15078,7 +14949,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -15107,7 +14978,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -15126,10 +14997,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -15142,7 +15010,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -15175,7 +15043,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -15204,7 +15072,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -15233,7 +15101,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -15272,7 +15140,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -15307,7 +15175,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -41694,8 +41566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K186" sqref="K186"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="L183" sqref="L183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>